<commit_message>
Changelog: - PCCs now have a type to better reconstruct where (in the project development timeline) the cost-prognosis is placed - trade.cost_group can now only be a main_cost_group (restricted via UI only as of now)
</commit_message>
<xml_diff>
--- a/templates/pcc_cost_groups_ov.xlsx
+++ b/templates/pcc_cost_groups_ov.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Google Drive\02 Arbeit\00 Fyuture\01 Learning\Python\00 Projekte\Kostenfortschreibung\Application\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3E47B5-294B-4196-AABB-CDC3686F9622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AC7C7B-ACDA-48AD-BE5A-F2CE72E863F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{1B4DD004-469C-4AD1-8C69-CAAF5867C2EC}"/>
+    <workbookView xWindow="10155" yWindow="1200" windowWidth="17310" windowHeight="12135" xr2:uid="{1B4DD004-469C-4AD1-8C69-CAAF5867C2EC}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
-    <t xml:space="preserve">Kostenschätzung  </t>
-  </si>
-  <si>
-    <t>Zusammenstellung der Kosten</t>
-  </si>
-  <si>
     <t>Kostengruppe</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>{pcc.name}</t>
+  </si>
+  <si>
+    <t>Kostenermittlung</t>
+  </si>
+  <si>
+    <t>Ermittelte Kosten</t>
   </si>
 </sst>
 </file>
@@ -427,171 +427,200 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -599,55 +628,24 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -657,40 +655,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -698,7 +695,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -713,55 +710,55 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1134,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E56C64C-23DC-4F82-99BB-43AB75BAE1E0}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,8 +1160,8 @@
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
-        <v>38</v>
+      <c r="A2" s="57" t="s">
+        <v>36</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1175,51 +1172,51 @@
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="43" t="s">
-        <v>0</v>
+      <c r="A4" s="42" t="s">
+        <v>40</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="A5" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
+      <c r="A9" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="13"/>
@@ -1229,96 +1226,96 @@
       <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="66"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="68"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="16" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
+      <c r="A18" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="4"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
@@ -1326,15 +1323,15 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="36" t="s">
-        <v>29</v>
+      <c r="A19" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="35" t="s">
+        <v>27</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
@@ -1342,15 +1339,15 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="27" t="s">
-        <v>40</v>
+      <c r="A20" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="26" t="s">
+        <v>38</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
@@ -1358,15 +1355,15 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
-        <v>9</v>
+      <c r="A21" s="44" t="s">
+        <v>7</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>7</v>
+      <c r="C21" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -1375,11 +1372,11 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
+      <c r="A23" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
@@ -1387,58 +1384,58 @@
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="41" t="s">
+      <c r="F24" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="42" t="s">
-        <v>12</v>
+      <c r="G24" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="41" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="57"/>
+      <c r="A27" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="56"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -1447,49 +1444,49 @@
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="52"/>
+      <c r="A28" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="51"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="52"/>
+      <c r="A29" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="51"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="55"/>
+      <c r="A30" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="54"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="60"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
       <c r="H31" s="13"/>
     </row>
   </sheetData>

</xml_diff>